<commit_message>
Add random forest classifier model
</commit_message>
<xml_diff>
--- a/model_performance_log.xlsx
+++ b/model_performance_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakog\Desktop\Class Stuff\Mod23_24 Project4\project4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data_Visualization_Analytics\Git_hub_projects\project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A98BED-D471-4BB4-B6E6-1991EF5A8D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02465DD8-796A-4607-BA9E-BDC7B28A9C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="4100" windowWidth="37800" windowHeight="19780" xr2:uid="{85667670-D47E-4548-8070-31D16966D4C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{85667670-D47E-4548-8070-31D16966D4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="project_4" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Layers</t>
   </si>
@@ -64,16 +64,36 @@
   </si>
   <si>
     <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>bank_marketing_random_forest</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,10 +131,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -129,8 +150,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -147,9 +170,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +210,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +316,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,129 +466,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BC030E-7C8C-44F5-A5B1-14414409E12A}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>0.91700000000000004</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>0.91900000000000004</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.91</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C9AED12A-68CE-4CB4-87B7-D963EC9DE5A2}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C7C77497-9A31-41DD-A60C-10415C1DE265}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{961831C5-438F-4D61-961E-B0694FFB448C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>